<commit_message>
add code convention and fix warnings
</commit_message>
<xml_diff>
--- a/content/codedesign/ResourceFormat.xlsx
+++ b/content/codedesign/ResourceFormat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DevVersioned\Tiki3\code\content\codedesign\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Development\tiki3_private\content\codedesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -167,9 +167,6 @@
     <t>enum { Pointer, String, ResourceLink } needs 2 bits</t>
   </si>
   <si>
-    <t>If AllocatorId is 0 this is the initialzation data detion</t>
-  </si>
-  <si>
     <t>OffsetInSection</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>SectionData = OffsetInFile + ( sizeof( ReferenceItem ) * ReferenceCount )</t>
+  </si>
+  <si>
+    <t>If AllocatorId is 0 this is the initialzation data section</t>
   </si>
 </sst>
 </file>
@@ -786,7 +786,7 @@
   <dimension ref="B1:J42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +804,7 @@
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -812,7 +812,7 @@
       <c r="F2" s="26"/>
       <c r="G2" s="25"/>
       <c r="I2" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J2" s="25"/>
     </row>
@@ -839,7 +839,7 @@
         <v>11</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J4" s="10">
         <v>1</v>
@@ -887,7 +887,7 @@
         <v>25</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -909,7 +909,7 @@
         <v>24</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -917,7 +917,7 @@
         <v>41</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -933,7 +933,7 @@
         <v>32</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -959,7 +959,7 @@
         <v>30</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -980,10 +980,10 @@
       </c>
       <c r="G10" s="2"/>
       <c r="I10" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
@@ -1007,7 +1007,7 @@
         <v>30</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1026,10 +1026,10 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="I12" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
         <v>24</v>
       </c>
       <c r="J13" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
@@ -1073,7 +1073,7 @@
         <v>32</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1095,7 +1095,7 @@
         <v>41</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
@@ -1117,15 +1117,15 @@
         <v>30</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I17" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J17" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
@@ -1141,7 +1141,7 @@
         <v>30</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1164,10 +1164,10 @@
         <v>23</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J19" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
@@ -1185,13 +1185,13 @@
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="I20" s="18" t="s">
         <v>30</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1212,10 +1212,10 @@
         <v>28</v>
       </c>
       <c r="I21" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
@@ -1265,7 +1265,7 @@
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -1319,7 +1319,7 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>6</v>
@@ -1332,12 +1332,12 @@
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>6</v>

</xml_diff>